<commit_message>
completed the transformer saturation example in ATP with a 500 km line and realistic line resistance
</commit_message>
<xml_diff>
--- a/cim/raw/XfmrSat.xlsx
+++ b/cim/raw/XfmrSat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\emthub\cim\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348271F7-0EB8-466C-A47B-ADF716E297C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B111EA4-60AF-4379-9668-D28C5C485AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="930" windowWidth="20040" windowHeight="19160" xr2:uid="{57A74BFE-98E6-4162-8EA1-6CBD6A5611BD}"/>
+    <workbookView xWindow="6900" yWindow="1480" windowWidth="23500" windowHeight="19160" xr2:uid="{57A74BFE-98E6-4162-8EA1-6CBD6A5611BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -203,11 +203,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -547,7 +546,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>300000</v>
+        <v>500000</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
@@ -612,7 +611,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2.0000000000000002E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
@@ -654,7 +653,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6.0000000000000002E-5</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="D10" t="s">
         <v>36</v>
@@ -685,7 +684,7 @@
       </c>
       <c r="B14">
         <f>B7*LineLength</f>
-        <v>6.0000000000000009</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -712,7 +711,7 @@
       </c>
       <c r="B17">
         <f>B10*LineLength</f>
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -737,9 +736,9 @@
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21">
         <f>B15*Omega*LineLength</f>
-        <v>113.1</v>
+        <v>188.5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -748,7 +747,7 @@
       </c>
       <c r="B22" s="1">
         <f>B16*Omega*LineLength</f>
-        <v>1.2566666666666668E-3</v>
+        <v>2.0944444444444448E-3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -757,7 +756,7 @@
       </c>
       <c r="B23" s="1">
         <f>B18*Omega*LineLength</f>
-        <v>452.4</v>
+        <v>754</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -766,7 +765,7 @@
       </c>
       <c r="B24" s="1">
         <f>B19*Omega*LineLength</f>
-        <v>7.0687500000000004E-4</v>
+        <v>1.1781249999999999E-3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -775,7 +774,7 @@
       </c>
       <c r="B26" s="1">
         <f>kVbase*kVbase*B22</f>
-        <v>149.57475000000002</v>
+        <v>249.29125000000005</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -784,34 +783,34 @@
       </c>
       <c r="B27" s="1">
         <f>kVbase*kVbase*B24</f>
-        <v>84.135796875000011</v>
+        <v>140.22632812499998</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <f>B14/Zbase</f>
-        <v>5.0409577819785769E-3</v>
+        <v>1.6803192606595255E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <f>B21/Zbase</f>
-        <v>9.5022054190296149E-2</v>
+        <v>0.15837009031716026</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <f>B26/MVAbase</f>
-        <v>1.4957475000000002</v>
+        <v>2.4929125000000005</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -820,7 +819,7 @@
       </c>
       <c r="B33">
         <f>B17/Zbase</f>
-        <v>1.5122873345935728E-2</v>
+        <v>3.3606385213190509E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -829,7 +828,7 @@
       </c>
       <c r="B34" s="1">
         <f>B23/Zbase</f>
-        <v>0.38008821676118459</v>
+        <v>0.63348036126864105</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -838,7 +837,7 @@
       </c>
       <c r="B35" s="1">
         <f>B27/MVAbase</f>
-        <v>0.84135796875000013</v>
+        <v>1.4022632812499998</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -847,7 +846,7 @@
       </c>
       <c r="B37">
         <f>1609*B21/LineLength</f>
-        <v>0.60659299999999994</v>
+        <v>0.60659300000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>